<commit_message>
updated testng-All and pom.xml to the default state
</commit_message>
<xml_diff>
--- a/test-data/TestData_R4R.xlsx
+++ b/test-data/TestData_R4R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1944D5D0-AA4D-4343-A2ED-714873F3802B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BA84DE0E-5734-4402-B954-BD7434043394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>C122614</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Detecting Mechanism of Action based Network Dysregulation (DeMAND)</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>tissue</t>
   </si>
 </sst>
 </file>
@@ -478,37 +484,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="62.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="4" customWidth="1"/>
     <col min="9" max="9" width="10" style="4" customWidth="1"/>
-    <col min="10" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
+    <col min="10" max="13" width="9.1796875" style="1"/>
+    <col min="14" max="14" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="1"/>
     <col min="18" max="18" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.1796875" style="1"/>
+    <col min="21" max="21" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="23" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -533,7 +539,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -551,7 +557,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -568,7 +574,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -582,6 +591,11 @@
         <v>17</v>
       </c>
       <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>